<commit_message>
cambios menores al placeholder telefono y carga de datos del sun
</commit_message>
<xml_diff>
--- a/www/public_ftp/iepe/storage/datos_sun/datos_sun.xlsx
+++ b/www/public_ftp/iepe/storage/datos_sun/datos_sun.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>ORIENTACION</t>
   </si>
@@ -123,21 +123,35 @@
   </si>
   <si>
     <t>Geovánni</t>
+  </si>
+  <si>
+    <t>Rodriguel</t>
+  </si>
+  <si>
+    <t>Mañoso</t>
+  </si>
+  <si>
+    <t>Güsanññño</t>
+  </si>
+  <si>
+    <t>Spenq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -197,12 +211,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,10 +241,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -525,6 +543,76 @@
         <v>2016</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1324354654</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>33238</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>41694</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>33238</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>41694</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>2014</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>